<commit_message>
populate all data form xlsx
</commit_message>
<xml_diff>
--- a/solucion_videos/videos/management/commands/import.xlsx
+++ b/solucion_videos/videos/management/commands/import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yajhaira.sanchez\proyectos_yurley\dp4_proyecto\solucion_videos\videos\management\commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{659DAEEA-BFD4-4767-9885-125FDA955F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCD2C67-A158-4102-81C7-6E3DD0C202AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{93B8CA32-BFD8-429D-B873-EC37D4CE600D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>titulo</t>
   </si>
@@ -43,14 +43,202 @@
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>titulo1</t>
+  </si>
+  <si>
+    <t>titulo2</t>
+  </si>
+  <si>
+    <t>titulo3</t>
+  </si>
+  <si>
+    <t>titulo4</t>
+  </si>
+  <si>
+    <t>titulo5</t>
+  </si>
+  <si>
+    <t>titulo6</t>
+  </si>
+  <si>
+    <t>titulo7</t>
+  </si>
+  <si>
+    <t>titulo8</t>
+  </si>
+  <si>
+    <t>titulo9</t>
+  </si>
+  <si>
+    <t>titulo10</t>
+  </si>
+  <si>
+    <t>titulo11</t>
+  </si>
+  <si>
+    <t>titulo12</t>
+  </si>
+  <si>
+    <t>titulo13</t>
+  </si>
+  <si>
+    <t>titulo14</t>
+  </si>
+  <si>
+    <t>titulo15</t>
+  </si>
+  <si>
+    <t>titulo16</t>
+  </si>
+  <si>
+    <t>titulo17</t>
+  </si>
+  <si>
+    <t>titulo18</t>
+  </si>
+  <si>
+    <t>titulo19</t>
+  </si>
+  <si>
+    <t>titulo20</t>
+  </si>
+  <si>
+    <t>titulo21</t>
+  </si>
+  <si>
+    <t>titulo22</t>
+  </si>
+  <si>
+    <t>titulo23</t>
+  </si>
+  <si>
+    <t>titulo24</t>
+  </si>
+  <si>
+    <t>titulo25</t>
+  </si>
+  <si>
+    <t>titulo26</t>
+  </si>
+  <si>
+    <t>titulo27</t>
+  </si>
+  <si>
+    <t>titulo28</t>
+  </si>
+  <si>
+    <t>titulo29</t>
+  </si>
+  <si>
+    <t>descripcion1</t>
+  </si>
+  <si>
+    <t>descripcion2</t>
+  </si>
+  <si>
+    <t>descripcion3</t>
+  </si>
+  <si>
+    <t>descripcion4</t>
+  </si>
+  <si>
+    <t>descripcion5</t>
+  </si>
+  <si>
+    <t>descripcion6</t>
+  </si>
+  <si>
+    <t>descripcion7</t>
+  </si>
+  <si>
+    <t>descripcion8</t>
+  </si>
+  <si>
+    <t>descripcion9</t>
+  </si>
+  <si>
+    <t>descripcion10</t>
+  </si>
+  <si>
+    <t>descripcion11</t>
+  </si>
+  <si>
+    <t>descripcion12</t>
+  </si>
+  <si>
+    <t>descripcion13</t>
+  </si>
+  <si>
+    <t>descripcion14</t>
+  </si>
+  <si>
+    <t>descripcion15</t>
+  </si>
+  <si>
+    <t>descripcion16</t>
+  </si>
+  <si>
+    <t>descripcion17</t>
+  </si>
+  <si>
+    <t>descripcion18</t>
+  </si>
+  <si>
+    <t>descripcion19</t>
+  </si>
+  <si>
+    <t>descripcion20</t>
+  </si>
+  <si>
+    <t>descripcion21</t>
+  </si>
+  <si>
+    <t>descripcion22</t>
+  </si>
+  <si>
+    <t>descripcion23</t>
+  </si>
+  <si>
+    <t>descripcion24</t>
+  </si>
+  <si>
+    <t>descripcion25</t>
+  </si>
+  <si>
+    <t>descripcion26</t>
+  </si>
+  <si>
+    <t>descripcion27</t>
+  </si>
+  <si>
+    <t>descripcion28</t>
+  </si>
+  <si>
+    <t>descripcion29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,8 +266,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,13 +583,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832112E0-1657-4875-8C11-3C33237FEEB0}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -414,286 +606,286 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -701,10 +893,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -712,10 +904,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -723,27 +915,17 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>